<commit_message>
Updated and cleaned data file
</commit_message>
<xml_diff>
--- a/responses_pilot/faulty ids.xlsx
+++ b/responses_pilot/faulty ids.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anmavrol/Desktop/ccstudy/responses_pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B45A02F-60A4-1445-997D-D2BF85CBA68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62D20E5-996B-5C4C-A726-7C9D005405AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="900" windowWidth="25040" windowHeight="13820" xr2:uid="{39FDF28C-FF83-C94B-BB71-C66BCDF62F55}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -67,12 +67,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,13 +388,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C1A127D-8C30-C04B-BE3F-B4757A31F8AB}">
-  <dimension ref="A1:A582"/>
+  <dimension ref="A1:A674"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A567" workbookViewId="0">
-      <selection activeCell="A582" sqref="A582"/>
+    <sheetView tabSelected="1" topLeftCell="A663" workbookViewId="0">
+      <selection activeCell="A674" sqref="A674"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.5" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
@@ -596,12 +600,12 @@
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="A41" s="2">
         <v>12653689744</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="A42" s="2">
         <v>12653648893</v>
       </c>
     </row>
@@ -3296,13 +3300,473 @@
       </c>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A581">
+      <c r="A581" s="2">
         <v>12273976395</v>
       </c>
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A582">
+      <c r="A582" s="2">
         <v>12281806763</v>
+      </c>
+    </row>
+    <row r="583" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A583" s="2">
+        <v>12900612745</v>
+      </c>
+    </row>
+    <row r="584" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A584" s="2">
+        <v>12900601934</v>
+      </c>
+    </row>
+    <row r="585" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A585" s="2">
+        <v>12900586917</v>
+      </c>
+    </row>
+    <row r="586" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A586" s="2">
+        <v>12900566978</v>
+      </c>
+    </row>
+    <row r="587" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A587" s="2">
+        <v>12900543510</v>
+      </c>
+    </row>
+    <row r="588" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A588" s="2">
+        <v>12900511357</v>
+      </c>
+    </row>
+    <row r="589" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A589" s="2">
+        <v>12900463211</v>
+      </c>
+    </row>
+    <row r="590" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A590" s="2">
+        <v>12900420036</v>
+      </c>
+    </row>
+    <row r="591" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A591" s="2">
+        <v>12900369194</v>
+      </c>
+    </row>
+    <row r="592" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A592" s="2">
+        <v>12900190549</v>
+      </c>
+    </row>
+    <row r="593" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A593" s="2">
+        <v>12900169901</v>
+      </c>
+    </row>
+    <row r="594" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A594" s="2">
+        <v>12900149072</v>
+      </c>
+    </row>
+    <row r="595" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A595" s="2">
+        <v>12900114171</v>
+      </c>
+    </row>
+    <row r="596" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A596" s="2">
+        <v>12899213448</v>
+      </c>
+    </row>
+    <row r="597" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A597" s="2">
+        <v>12899134862</v>
+      </c>
+    </row>
+    <row r="598" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A598" s="2">
+        <v>12898964027</v>
+      </c>
+    </row>
+    <row r="599" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A599" s="2">
+        <v>12898642970</v>
+      </c>
+    </row>
+    <row r="600" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A600" s="2">
+        <v>12898365222</v>
+      </c>
+    </row>
+    <row r="601" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A601" s="2">
+        <v>12898343328</v>
+      </c>
+    </row>
+    <row r="602" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A602" s="2">
+        <v>12898343247</v>
+      </c>
+    </row>
+    <row r="603" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A603" s="2">
+        <v>12898343276</v>
+      </c>
+    </row>
+    <row r="604" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A604" s="2">
+        <v>12898343271</v>
+      </c>
+    </row>
+    <row r="605" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A605" s="2">
+        <v>12898343265</v>
+      </c>
+    </row>
+    <row r="606" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A606" s="2">
+        <v>12898343258</v>
+      </c>
+    </row>
+    <row r="607" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A607" s="2">
+        <v>12898343245</v>
+      </c>
+    </row>
+    <row r="608" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A608" s="2">
+        <v>12898343252</v>
+      </c>
+    </row>
+    <row r="609" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A609" s="2">
+        <v>12898343246</v>
+      </c>
+    </row>
+    <row r="610" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A610" s="2">
+        <v>12898343257</v>
+      </c>
+    </row>
+    <row r="611" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A611" s="2">
+        <v>12898343275</v>
+      </c>
+    </row>
+    <row r="612" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A612" s="2">
+        <v>12898343249</v>
+      </c>
+    </row>
+    <row r="613" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A613" s="2">
+        <v>12898343260</v>
+      </c>
+    </row>
+    <row r="614" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A614" s="2">
+        <v>12898343250</v>
+      </c>
+    </row>
+    <row r="615" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A615" s="2">
+        <v>12898343283</v>
+      </c>
+    </row>
+    <row r="616" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A616" s="2">
+        <v>12898343264</v>
+      </c>
+    </row>
+    <row r="617" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A617" s="2">
+        <v>12898343337</v>
+      </c>
+    </row>
+    <row r="618" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A618" s="2">
+        <v>12898346382</v>
+      </c>
+    </row>
+    <row r="619" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A619" s="2">
+        <v>12898330068</v>
+      </c>
+    </row>
+    <row r="620" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A620" s="2">
+        <v>12871365441</v>
+      </c>
+    </row>
+    <row r="621" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A621" s="2">
+        <v>12871365340</v>
+      </c>
+    </row>
+    <row r="622" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A622" s="2">
+        <v>12871365208</v>
+      </c>
+    </row>
+    <row r="623" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A623" s="2">
+        <v>12870703808</v>
+      </c>
+    </row>
+    <row r="624" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A624" s="2">
+        <v>12870608853</v>
+      </c>
+    </row>
+    <row r="625" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A625" s="2">
+        <v>12870608644</v>
+      </c>
+    </row>
+    <row r="626" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A626" s="2">
+        <v>12870608540</v>
+      </c>
+    </row>
+    <row r="627" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A627" s="2">
+        <v>12870608412</v>
+      </c>
+    </row>
+    <row r="628" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A628" s="2">
+        <v>12870605393</v>
+      </c>
+    </row>
+    <row r="629" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A629" s="2">
+        <v>12870605319</v>
+      </c>
+    </row>
+    <row r="630" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A630" s="2">
+        <v>12870605251</v>
+      </c>
+    </row>
+    <row r="631" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A631" s="2">
+        <v>12870605086</v>
+      </c>
+    </row>
+    <row r="632" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A632" s="2">
+        <v>12870605168</v>
+      </c>
+    </row>
+    <row r="633" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A633" s="2">
+        <v>12870608901</v>
+      </c>
+    </row>
+    <row r="634" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A634" s="2">
+        <v>12870602990</v>
+      </c>
+    </row>
+    <row r="635" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A635" s="2">
+        <v>12870570962</v>
+      </c>
+    </row>
+    <row r="636" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A636" s="2">
+        <v>12870563163</v>
+      </c>
+    </row>
+    <row r="637" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A637" s="2">
+        <v>12870562919</v>
+      </c>
+    </row>
+    <row r="638" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A638" s="2">
+        <v>12870562798</v>
+      </c>
+    </row>
+    <row r="639" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A639" s="2">
+        <v>12870562628</v>
+      </c>
+    </row>
+    <row r="640" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A640" s="2">
+        <v>12870562509</v>
+      </c>
+    </row>
+    <row r="641" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A641" s="2">
+        <v>12870575866</v>
+      </c>
+    </row>
+    <row r="642" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A642" s="2">
+        <v>12870535188</v>
+      </c>
+    </row>
+    <row r="643" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A643" s="2">
+        <v>12870534563</v>
+      </c>
+    </row>
+    <row r="644" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A644" s="2">
+        <v>12870536330</v>
+      </c>
+    </row>
+    <row r="645" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A645" s="2">
+        <v>12870535776</v>
+      </c>
+    </row>
+    <row r="646" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A646" s="2">
+        <v>12870554968</v>
+      </c>
+    </row>
+    <row r="647" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A647" s="2">
+        <v>12870534440</v>
+      </c>
+    </row>
+    <row r="648" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A648" s="2">
+        <v>12870487929</v>
+      </c>
+    </row>
+    <row r="649" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A649" s="2">
+        <v>12870538153</v>
+      </c>
+    </row>
+    <row r="650" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A650" s="2">
+        <v>12870538027</v>
+      </c>
+    </row>
+    <row r="651" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A651" s="2">
+        <v>12870537898</v>
+      </c>
+    </row>
+    <row r="652" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A652" s="2">
+        <v>12870537764</v>
+      </c>
+    </row>
+    <row r="653" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A653" s="2">
+        <v>12870537662</v>
+      </c>
+    </row>
+    <row r="654" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A654" s="2">
+        <v>12870487102</v>
+      </c>
+    </row>
+    <row r="655" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A655" s="2">
+        <v>12870486428</v>
+      </c>
+    </row>
+    <row r="656" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A656" s="2">
+        <v>12870487774</v>
+      </c>
+    </row>
+    <row r="657" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A657" s="2">
+        <v>12870564403</v>
+      </c>
+    </row>
+    <row r="658" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A658" s="2">
+        <v>12870532864</v>
+      </c>
+    </row>
+    <row r="659" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A659" s="2">
+        <v>12870543836</v>
+      </c>
+    </row>
+    <row r="660" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A660" s="2">
+        <v>12870506467</v>
+      </c>
+    </row>
+    <row r="661" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A661" s="2">
+        <v>12870484493</v>
+      </c>
+    </row>
+    <row r="662" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A662" s="2">
+        <v>12870514486</v>
+      </c>
+    </row>
+    <row r="663" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A663" s="2">
+        <v>12870514132</v>
+      </c>
+    </row>
+    <row r="664" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A664" s="2">
+        <v>12870489185</v>
+      </c>
+    </row>
+    <row r="665" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A665" s="2">
+        <v>12870483349</v>
+      </c>
+    </row>
+    <row r="666" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A666" s="2">
+        <v>12870460246</v>
+      </c>
+    </row>
+    <row r="667" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A667" s="2">
+        <v>12741081295</v>
+      </c>
+    </row>
+    <row r="668" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A668" s="2">
+        <v>12720598465</v>
+      </c>
+    </row>
+    <row r="669" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A669" s="2">
+        <v>12720595503</v>
+      </c>
+    </row>
+    <row r="670" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A670" s="2">
+        <v>12676540645</v>
+      </c>
+    </row>
+    <row r="671" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A671" s="2">
+        <v>12568164440</v>
+      </c>
+    </row>
+    <row r="672" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A672" s="2">
+        <v>12707383608</v>
+      </c>
+    </row>
+    <row r="673" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A673" s="2">
+        <v>12706315010</v>
+      </c>
+    </row>
+    <row r="674" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A674" s="3">
+        <v>12869063756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>